<commit_message>
minor updates late 2024
</commit_message>
<xml_diff>
--- a/db/MoleWeights.xlsx
+++ b/db/MoleWeights.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elars\Desktop\Yale School Stuff\EPS 529 - Geodynamics\Project continued\MORedox_2023_v3\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50ED738B-0B9A-4215-9ABD-9D92BEFDB704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{294D540F-7892-4EF1-A1CE-950267B02135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="23657" windowHeight="15240" activeTab="5" xr2:uid="{47A84D43-22DB-204C-98DE-F7496EE65383}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="24892" windowHeight="14914" firstSheet="2" activeTab="7" xr2:uid="{47A84D43-22DB-204C-98DE-F7496EE65383}"/>
   </bookViews>
   <sheets>
     <sheet name="Rubie11_Emantle" sheetId="11" r:id="rId1"/>
@@ -19,12 +19,14 @@
     <sheet name="ImpEarly_core" sheetId="15" r:id="rId4"/>
     <sheet name="ImpLate_mantle" sheetId="6" r:id="rId5"/>
     <sheet name="ImpLate_core" sheetId="14" r:id="rId6"/>
-    <sheet name="metal" sheetId="12" r:id="rId7"/>
-    <sheet name="Deng20" sheetId="1" r:id="rId8"/>
-    <sheet name="Armstrong19" sheetId="2" r:id="rId9"/>
-    <sheet name="Hirsch22" sheetId="3" r:id="rId10"/>
-    <sheet name="EarthEarly" sheetId="4" r:id="rId11"/>
-    <sheet name="EarthLate" sheetId="7" r:id="rId12"/>
+    <sheet name="ImpMid_mantle" sheetId="16" r:id="rId7"/>
+    <sheet name="ImpMid_core" sheetId="17" r:id="rId8"/>
+    <sheet name="metal" sheetId="12" r:id="rId9"/>
+    <sheet name="Deng20" sheetId="1" r:id="rId10"/>
+    <sheet name="Armstrong19" sheetId="2" r:id="rId11"/>
+    <sheet name="Hirsch22" sheetId="3" r:id="rId12"/>
+    <sheet name="EarthEarly" sheetId="4" r:id="rId13"/>
+    <sheet name="EarthLate" sheetId="7" r:id="rId14"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -45,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="34">
   <si>
     <t>SiO2</t>
   </si>
@@ -1615,6 +1617,373 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D605C485-1DC2-CE40-93E0-F6D4262E732D}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D26" sqref="D26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>45.49</v>
+      </c>
+      <c r="C2">
+        <v>60.073499999999996</v>
+      </c>
+      <c r="D2">
+        <v>60.084000000000003</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0.2</v>
+      </c>
+      <c r="C3">
+        <v>79.055000000000007</v>
+      </c>
+      <c r="D3">
+        <v>79.864999999999995</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4.45</v>
+      </c>
+      <c r="C4">
+        <v>50.971000000000004</v>
+      </c>
+      <c r="D4">
+        <v>101.961</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>75.986999999999995</v>
+      </c>
+      <c r="D5">
+        <v>151.989</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>8.1</v>
+      </c>
+      <c r="C6">
+        <v>71.838999999999999</v>
+      </c>
+      <c r="D6">
+        <v>71.843999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>70.932000000000002</v>
+      </c>
+      <c r="D7">
+        <v>70.936999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>37.799999999999997</v>
+      </c>
+      <c r="C8">
+        <v>40.298999999999999</v>
+      </c>
+      <c r="D8">
+        <v>40.304000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>58.9634</v>
+      </c>
+      <c r="D9">
+        <v>74.691999999999993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>3.55</v>
+      </c>
+      <c r="C10">
+        <v>56.072000000000003</v>
+      </c>
+      <c r="D10">
+        <v>56.076999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>0.36</v>
+      </c>
+      <c r="C11">
+        <v>30.986799999999999</v>
+      </c>
+      <c r="D11">
+        <v>61.972000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="C12">
+        <v>47.094999999999999</v>
+      </c>
+      <c r="D12">
+        <v>94.194999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="C13">
+        <v>70.959000000000003</v>
+      </c>
+      <c r="D13">
+        <v>141.94300000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F6B0B9-3302-493B-9F61-2729263CC03A}">
+  <dimension ref="A1:G13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>57.3</v>
+      </c>
+      <c r="C2">
+        <v>60.073499999999996</v>
+      </c>
+      <c r="G2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>79.055000000000007</v>
+      </c>
+      <c r="G3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>14.8</v>
+      </c>
+      <c r="C4">
+        <v>50.971000000000004</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>75.986999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>9.4</v>
+      </c>
+      <c r="C6">
+        <v>71.838999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>70.932000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>2.1</v>
+      </c>
+      <c r="C8">
+        <v>40.298999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>58.9634</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>7.4</v>
+      </c>
+      <c r="C10">
+        <v>56.072000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>4.4000000000000004</v>
+      </c>
+      <c r="C11">
+        <v>30.986799999999999</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="C12">
+        <v>47.094999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <v>70.959000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5146B3F2-5D51-4479-B498-CD00EDF9B2C3}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -1776,7 +2145,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{581EC8AC-69E9-401A-A66F-7E71B38645AD}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -1935,7 +2304,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A921F10-46BC-4155-A64F-34FE739E62CD}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -2798,7 +3167,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J24" sqref="J24"/>
+      <selection sqref="A1:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -3002,7 +3371,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1:D2"/>
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -3108,7 +3477,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+      <selection sqref="A1:D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -3311,8 +3680,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6730E3DD-1B24-416B-963B-8536D03899DF}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
@@ -3414,6 +3783,326 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76A89F29-FBE7-480D-AC22-56354C806ACA}">
+  <dimension ref="A1:D13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>46.53</v>
+      </c>
+      <c r="C2">
+        <f>60.084</f>
+        <v>60.084000000000003</v>
+      </c>
+      <c r="D2">
+        <v>60.084000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <f>79.865</f>
+        <v>79.864999999999995</v>
+      </c>
+      <c r="D3">
+        <v>79.864999999999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>4.4800000000000004</v>
+      </c>
+      <c r="C4">
+        <f>D4/2</f>
+        <v>50.980499999999999</v>
+      </c>
+      <c r="D4">
+        <v>101.961</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <f>D5/2</f>
+        <v>75.994500000000002</v>
+      </c>
+      <c r="D5">
+        <v>151.989</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
+        <v>8.89</v>
+      </c>
+      <c r="C6">
+        <v>71.843999999999994</v>
+      </c>
+      <c r="D6">
+        <v>71.843999999999994</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>70.936999999999998</v>
+      </c>
+      <c r="D7">
+        <v>70.936999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>36.450000000000003</v>
+      </c>
+      <c r="C8">
+        <v>40.304000000000002</v>
+      </c>
+      <c r="D8">
+        <v>40.304000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>74.691999999999993</v>
+      </c>
+      <c r="D9">
+        <v>74.691999999999993</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10">
+        <v>3.64</v>
+      </c>
+      <c r="C10">
+        <v>56.076999999999998</v>
+      </c>
+      <c r="D10">
+        <v>56.076999999999998</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11">
+        <v>0</v>
+      </c>
+      <c r="C11">
+        <f>D11/2</f>
+        <v>30.986000000000001</v>
+      </c>
+      <c r="D11">
+        <v>61.972000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <f>D12/2</f>
+        <v>47.097499999999997</v>
+      </c>
+      <c r="D12">
+        <v>94.194999999999993</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13">
+        <v>0</v>
+      </c>
+      <c r="C13">
+        <f>D13/2</f>
+        <v>70.971500000000006</v>
+      </c>
+      <c r="D13">
+        <v>141.94300000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14E6418D-1121-49F2-BC08-7B9502241B45}">
+  <dimension ref="A1:I24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J17" sqref="J17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2">
+        <v>87.96</v>
+      </c>
+      <c r="C2">
+        <v>55.844999999999999</v>
+      </c>
+      <c r="D2">
+        <v>0.81</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3">
+        <v>6.61</v>
+      </c>
+      <c r="C3">
+        <v>58.692999999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4">
+        <v>0.3</v>
+      </c>
+      <c r="C4">
+        <v>58.933</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5">
+        <v>4.8</v>
+      </c>
+      <c r="C5">
+        <v>28.085000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6">
+        <v>0.33</v>
+      </c>
+      <c r="C6">
+        <v>15.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7">
+        <v>0.52</v>
+      </c>
+      <c r="C7">
+        <v>51.996000000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05D74315-7BB2-43C4-85AC-12998C31C28C}">
   <dimension ref="A1:E8"/>
   <sheetViews>
@@ -3544,371 +4233,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D605C485-1DC2-CE40-93E0-F6D4262E732D}">
-  <dimension ref="A1:G13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>45.49</v>
-      </c>
-      <c r="C2">
-        <v>60.073499999999996</v>
-      </c>
-      <c r="D2">
-        <v>60.084000000000003</v>
-      </c>
-      <c r="G2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>0.2</v>
-      </c>
-      <c r="C3">
-        <v>79.055000000000007</v>
-      </c>
-      <c r="D3">
-        <v>79.864999999999995</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>4.45</v>
-      </c>
-      <c r="C4">
-        <v>50.971000000000004</v>
-      </c>
-      <c r="D4">
-        <v>101.961</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>75.986999999999995</v>
-      </c>
-      <c r="D5">
-        <v>151.989</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>8.1</v>
-      </c>
-      <c r="C6">
-        <v>71.838999999999999</v>
-      </c>
-      <c r="D6">
-        <v>71.843999999999994</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>70.932000000000002</v>
-      </c>
-      <c r="D7">
-        <v>70.936999999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>37.799999999999997</v>
-      </c>
-      <c r="C8">
-        <v>40.298999999999999</v>
-      </c>
-      <c r="D8">
-        <v>40.304000000000002</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>58.9634</v>
-      </c>
-      <c r="D9">
-        <v>74.691999999999993</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>3.55</v>
-      </c>
-      <c r="C10">
-        <v>56.072000000000003</v>
-      </c>
-      <c r="D10">
-        <v>56.076999999999998</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>0.36</v>
-      </c>
-      <c r="C11">
-        <v>30.986799999999999</v>
-      </c>
-      <c r="D11">
-        <v>61.972000000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>2.9000000000000001E-2</v>
-      </c>
-      <c r="C12">
-        <v>47.094999999999999</v>
-      </c>
-      <c r="D12">
-        <v>94.194999999999993</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>2.1000000000000001E-2</v>
-      </c>
-      <c r="C13">
-        <v>70.959000000000003</v>
-      </c>
-      <c r="D13">
-        <v>141.94300000000001</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10F6B0B9-3302-493B-9F61-2729263CC03A}">
-  <dimension ref="A1:G13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="15.9" x14ac:dyDescent="0.45"/>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>57.3</v>
-      </c>
-      <c r="C2">
-        <v>60.073499999999996</v>
-      </c>
-      <c r="G2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>79.055000000000007</v>
-      </c>
-      <c r="G3" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4">
-        <v>14.8</v>
-      </c>
-      <c r="C4">
-        <v>50.971000000000004</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5">
-        <v>0</v>
-      </c>
-      <c r="C5">
-        <v>75.986999999999995</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6">
-        <v>9.4</v>
-      </c>
-      <c r="C6">
-        <v>71.838999999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A7" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7">
-        <v>0</v>
-      </c>
-      <c r="C7">
-        <v>70.932000000000002</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>5</v>
-      </c>
-      <c r="B8">
-        <v>2.1</v>
-      </c>
-      <c r="C8">
-        <v>40.298999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A9" t="s">
-        <v>10</v>
-      </c>
-      <c r="B9">
-        <v>0</v>
-      </c>
-      <c r="C9">
-        <v>58.9634</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10">
-        <v>7.4</v>
-      </c>
-      <c r="C10">
-        <v>56.072000000000003</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>4.4000000000000004</v>
-      </c>
-      <c r="C11">
-        <v>30.986799999999999</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="C12">
-        <v>47.094999999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
-      </c>
-      <c r="C13">
-        <v>70.959000000000003</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>